<commit_message>
add code, results and readme
</commit_message>
<xml_diff>
--- a/data/example_meta-metrics_calculation.xlsx
+++ b/data/example_meta-metrics_calculation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranji\UBC_Coursework\Projects\Analytics_Dashboard\mls-goals-added\goals-added\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C7163031-64C3-48BF-A50F-1E80981AB1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C04998-2990-4DF1-838F-8F671BC42AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example_meta_metrics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -139,10 +139,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -853,9 +853,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -867,18 +867,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="25" xfId="33" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="16" fillId="23" borderId="26" xfId="33" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="23" xfId="33" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="16" fillId="23" borderId="24" xfId="33" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="21" xfId="32" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="22" borderId="22" xfId="32" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="23" borderId="24" xfId="33" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="21" xfId="32" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="22" borderId="22" xfId="32" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="14" xfId="29" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1261,11 +1260,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,40 +1311,40 @@
     </row>
     <row r="4" spans="2:16" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="27" t="s">
+      <c r="B5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="27" t="s">
+      <c r="F5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="27" t="s">
+      <c r="J5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P5" s="27" t="s">
+      <c r="N5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="26" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1426,78 +1425,78 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="20">
-        <v>1</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="B8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="D8" s="20">
         <v>2020</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="20">
-        <v>1</v>
-      </c>
-      <c r="H8" s="21">
+      <c r="F8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="19">
+        <v>1</v>
+      </c>
+      <c r="H8" s="20">
         <v>2020</v>
       </c>
-      <c r="J8" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="20">
-        <v>1</v>
-      </c>
-      <c r="L8" s="21">
+      <c r="J8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="19">
+        <v>1</v>
+      </c>
+      <c r="L8" s="20">
         <v>2020</v>
       </c>
-      <c r="N8" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="O8" s="20">
-        <v>3</v>
-      </c>
-      <c r="P8" s="21">
+      <c r="N8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="19">
+        <v>3</v>
+      </c>
+      <c r="P8" s="20">
         <v>2020</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="20">
-        <v>1</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="20">
         <v>2020</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="20">
-        <v>1</v>
-      </c>
-      <c r="H9" s="21">
+      <c r="F9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="19">
+        <v>1</v>
+      </c>
+      <c r="H9" s="20">
         <v>2020</v>
       </c>
-      <c r="J9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="K9" s="20">
-        <v>1</v>
-      </c>
-      <c r="L9" s="21">
+      <c r="J9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="19">
+        <v>1</v>
+      </c>
+      <c r="L9" s="20">
         <v>2020</v>
       </c>
-      <c r="N9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="O9" s="20">
-        <v>1</v>
-      </c>
-      <c r="P9" s="21">
+      <c r="N9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="19">
+        <v>1</v>
+      </c>
+      <c r="P9" s="20">
         <v>2020</v>
       </c>
     </row>
@@ -1578,78 +1577,78 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="20">
-        <v>1</v>
-      </c>
-      <c r="D12" s="21">
+      <c r="B12" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20">
         <v>2021</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="20">
-        <v>1</v>
-      </c>
-      <c r="H12" s="21">
+      <c r="F12" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="19">
+        <v>1</v>
+      </c>
+      <c r="H12" s="20">
         <v>2021</v>
       </c>
-      <c r="J12" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="K12" s="20">
-        <v>1</v>
-      </c>
-      <c r="L12" s="21">
+      <c r="J12" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="19">
+        <v>1</v>
+      </c>
+      <c r="L12" s="20">
         <v>2021</v>
       </c>
-      <c r="N12" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="O12" s="20">
+      <c r="N12" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="19">
         <v>5</v>
       </c>
-      <c r="P12" s="21">
+      <c r="P12" s="20">
         <v>2021</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="20">
-        <v>1</v>
-      </c>
-      <c r="D13" s="21">
+      <c r="B13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="19">
+        <v>1</v>
+      </c>
+      <c r="D13" s="20">
         <v>2021</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="20">
-        <v>1</v>
-      </c>
-      <c r="H13" s="21">
+      <c r="F13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="19">
+        <v>1</v>
+      </c>
+      <c r="H13" s="20">
         <v>2021</v>
       </c>
-      <c r="J13" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" s="20">
-        <v>1</v>
-      </c>
-      <c r="L13" s="21">
+      <c r="J13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="19">
+        <v>1</v>
+      </c>
+      <c r="L13" s="20">
         <v>2021</v>
       </c>
-      <c r="N13" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="O13" s="20">
+      <c r="N13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" s="19">
         <v>2</v>
       </c>
-      <c r="P13" s="21">
+      <c r="P13" s="20">
         <v>2021</v>
       </c>
     </row>
@@ -1730,78 +1729,78 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="20">
-        <v>1</v>
-      </c>
-      <c r="D16" s="21">
+      <c r="B16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20">
         <v>2022</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="20">
-        <v>1</v>
-      </c>
-      <c r="H16" s="21">
+      <c r="F16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="19">
+        <v>1</v>
+      </c>
+      <c r="H16" s="20">
         <v>2022</v>
       </c>
-      <c r="J16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" s="20">
-        <v>1</v>
-      </c>
-      <c r="L16" s="21">
+      <c r="J16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="19">
+        <v>1</v>
+      </c>
+      <c r="L16" s="20">
         <v>2022</v>
       </c>
-      <c r="N16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="O16" s="20">
+      <c r="N16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O16" s="19">
         <v>2</v>
       </c>
-      <c r="P16" s="21">
+      <c r="P16" s="20">
         <v>2022</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="23">
-        <v>1</v>
-      </c>
-      <c r="D17" s="24">
+      <c r="B17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+      <c r="D17" s="23">
         <v>2022</v>
       </c>
-      <c r="F17" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="23">
-        <v>1</v>
-      </c>
-      <c r="H17" s="24">
+      <c r="F17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="22">
+        <v>1</v>
+      </c>
+      <c r="H17" s="23">
         <v>2022</v>
       </c>
-      <c r="J17" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="23">
-        <v>1</v>
-      </c>
-      <c r="L17" s="24">
+      <c r="J17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="22">
+        <v>1</v>
+      </c>
+      <c r="L17" s="23">
         <v>2022</v>
       </c>
-      <c r="N17" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="O17" s="23">
+      <c r="N17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="22">
         <v>2</v>
       </c>
-      <c r="P17" s="24">
+      <c r="P17" s="23">
         <v>2022</v>
       </c>
     </row>
@@ -1833,529 +1832,529 @@
     </row>
     <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="F21" s="11" t="s">
+      <c r="C21" s="7"/>
+      <c r="F21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="J21" s="11" t="s">
+      <c r="G21" s="7"/>
+      <c r="J21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K21" s="8"/>
-      <c r="N21" s="11" t="s">
+      <c r="K21" s="7"/>
+      <c r="N21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O21" s="8"/>
+      <c r="O21" s="7"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <f>_xlfn.VAR.P(C6:C7)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <f>_xlfn.VAR.P(G6:G7)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="J22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="9">
         <f>_xlfn.VAR.P(K6:K7)</f>
         <v>0</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="N22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O22" s="10">
+      <c r="O22" s="9">
         <f>_xlfn.VAR.P(O6:O7)</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <f>_xlfn.VAR.P(C8:C9)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="9">
         <f>_xlfn.VAR.P(G8:G9)</f>
         <v>0</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="J23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="9">
         <f>_xlfn.VAR.P(K8:K9)</f>
         <v>0</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="N23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O23" s="10">
+      <c r="O23" s="9">
         <f>_xlfn.VAR.P(O8:O9)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <f>AVERAGE(C22:C23)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="9">
         <f>AVERAGE(G22:G23)</f>
         <v>0</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="J24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="9">
         <f>AVERAGE(K22:K23)</f>
         <v>0</v>
       </c>
-      <c r="N24" s="9" t="s">
+      <c r="N24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O24" s="10">
+      <c r="O24" s="9">
         <f>AVERAGE(O22:O23)</f>
         <v>0.625</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="9">
         <f>_xlfn.VAR.P(C6:C9)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="9">
         <f>_xlfn.VAR.P(G6:G9)</f>
         <v>0.25</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="9">
         <f>_xlfn.VAR.P(K6:K9)</f>
         <v>0</v>
       </c>
-      <c r="N25" s="9" t="s">
+      <c r="N25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O25" s="10">
+      <c r="O25" s="9">
         <f>_xlfn.VAR.P(O6:O9)</f>
         <v>0.6875</v>
       </c>
     </row>
-    <row r="26" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="17" t="s">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="17">
         <f>1-((C24+$C$19)/(C25+$C$19))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="17">
         <f>1-((G24+$C$19)/(G25+$C$19))</f>
         <v>0.99601593625498008</v>
       </c>
-      <c r="J26" s="17" t="s">
+      <c r="J26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="17">
         <f>1-((K24+$C$19)/(K25+$C$19))</f>
         <v>0</v>
       </c>
-      <c r="N26" s="17" t="s">
+      <c r="N26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="O26" s="18">
+      <c r="O26" s="17">
         <f>1-((O24+$C$19)/(O25+$C$19))</f>
         <v>9.0777051561365285E-2</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="10"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="10"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="10"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="9"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="9"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="9">
         <f>_xlfn.VAR.P(C10:C11)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="9">
         <f>_xlfn.VAR.P(G10:G11)</f>
         <v>0.25</v>
       </c>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="9">
         <f>_xlfn.VAR.P(K10:K11)</f>
         <v>0</v>
       </c>
-      <c r="N28" s="9" t="s">
+      <c r="N28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="O28" s="10">
+      <c r="O28" s="9">
         <f>_xlfn.VAR.P(O10:O11)</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <f>_xlfn.VAR.P(C12:C13)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="9">
         <f>_xlfn.VAR.P(G12:G13)</f>
         <v>0</v>
       </c>
-      <c r="J29" s="9" t="s">
+      <c r="J29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="9">
         <f>_xlfn.VAR.P(K12:K13)</f>
         <v>0</v>
       </c>
-      <c r="N29" s="9" t="s">
+      <c r="N29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O29" s="10">
+      <c r="O29" s="9">
         <f>_xlfn.VAR.P(O12:O13)</f>
         <v>2.25</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <f>AVERAGE(C28:C29)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="9">
         <f>AVERAGE(G28:G29)</f>
         <v>0.125</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="J30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="9">
         <f>AVERAGE(K28:K29)</f>
         <v>0</v>
       </c>
-      <c r="N30" s="9" t="s">
+      <c r="N30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O30" s="10">
+      <c r="O30" s="9">
         <f>AVERAGE(O28:O29)</f>
         <v>1.625</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="9">
         <f>_xlfn.VAR.P(C10:C13)</f>
         <v>0</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="9">
         <f>_xlfn.VAR.P(G10:G13)</f>
         <v>1.6875</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="9">
         <f>_xlfn.VAR.P(K10:K13)</f>
         <v>0.25</v>
       </c>
-      <c r="N31" s="9" t="s">
+      <c r="N31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O31" s="10">
+      <c r="O31" s="9">
         <f>_xlfn.VAR.P(O10:O13)</f>
         <v>1.6875</v>
       </c>
     </row>
-    <row r="32" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="17" t="s">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="17">
         <f>1-((C30+$C$19)/(C31+$C$19))</f>
         <v>0</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="18">
+      <c r="G32" s="17">
         <f>1-((G30+$C$19)/(G31+$C$19))</f>
         <v>0.92537755404204913</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="J32" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="18">
+      <c r="K32" s="17">
         <f>1-((K30+$C$19)/(K31+$C$19))</f>
         <v>0.99601593625498008</v>
       </c>
-      <c r="N32" s="17" t="s">
+      <c r="N32" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="O32" s="18">
+      <c r="O32" s="17">
         <f>1-((O30+$C$19)/(O31+$C$19))</f>
         <v>3.7015102161682023E-2</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="10"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="10"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="10"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="9"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="9"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="9"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <f>_xlfn.VAR.P(C14:C15)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="9">
         <f>_xlfn.VAR.P(G14:G15)</f>
         <v>0.25</v>
       </c>
-      <c r="J34" s="9" t="s">
+      <c r="J34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K34" s="9">
         <f>_xlfn.VAR.P(K14:K15)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="9" t="s">
+      <c r="N34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="O34" s="10">
+      <c r="O34" s="9">
         <f>_xlfn.VAR.P(O14:O15)</f>
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="9">
         <f>_xlfn.VAR.P(C16:C17)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="9">
         <f>_xlfn.VAR.P(G16:G17)</f>
         <v>0</v>
       </c>
-      <c r="J35" s="9" t="s">
+      <c r="J35" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K35" s="9">
         <f>_xlfn.VAR.P(K16:K17)</f>
         <v>0</v>
       </c>
-      <c r="N35" s="9" t="s">
+      <c r="N35" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O35" s="10">
+      <c r="O35" s="9">
         <f>_xlfn.VAR.P(O16:O17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <f>AVERAGE(C34:C35)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="9">
         <f>AVERAGE(G34:G35)</f>
         <v>0.125</v>
       </c>
-      <c r="J36" s="9" t="s">
+      <c r="J36" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="9">
         <f>AVERAGE(K34:K35)</f>
         <v>0</v>
       </c>
-      <c r="N36" s="9" t="s">
+      <c r="N36" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="O36" s="10">
+      <c r="O36" s="9">
         <f>AVERAGE(O34:O35)</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="9">
         <f>_xlfn.VAR.P(C14:C17)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="9">
         <f>_xlfn.VAR.P(G14:G17)</f>
         <v>3.1875</v>
       </c>
-      <c r="J37" s="9" t="s">
+      <c r="J37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="9">
         <f>_xlfn.VAR.P(K14:K17)</f>
         <v>1</v>
       </c>
-      <c r="N37" s="9" t="s">
+      <c r="N37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O37" s="10">
+      <c r="O37" s="9">
         <f>_xlfn.VAR.P(O14:O17)</f>
         <v>5.5</v>
       </c>
     </row>
-    <row r="38" spans="2:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="s">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="17">
         <f>1-((C36+$C$19)/(C37+$C$19))</f>
         <v>0</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G38" s="17">
         <f>1-((G36+$C$19)/(G37+$C$19))</f>
         <v>0.96048298572996704</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="17">
         <f>1-((K36+$C$19)/(K37+$C$19))</f>
         <v>0.99900099900099903</v>
       </c>
-      <c r="N38" s="17" t="s">
+      <c r="N38" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="O38" s="18">
+      <c r="O38" s="17">
         <f>1-((O36+$C$19)/(O37+$C$19))</f>
         <v>0.18178512997636798</v>
       </c>
     </row>
     <row r="39" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="10"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="10"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="10"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="9"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="9"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="9"/>
     </row>
     <row r="40" spans="2:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="13">
         <f>AVERAGE(C26,C32,C38)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="F40" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="13">
         <f>AVERAGE(G26,G32,G38)</f>
         <v>0.96062549200899883</v>
       </c>
-      <c r="J40" s="13" t="s">
+      <c r="J40" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K40" s="14">
+      <c r="K40" s="13">
         <f>AVERAGE(K26,K32,K38)</f>
         <v>0.66500564508532634</v>
       </c>
-      <c r="N40" s="13" t="s">
+      <c r="N40" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="O40" s="14">
+      <c r="O40" s="13">
         <f>AVERAGE(O26,O32,O38)</f>
         <v>0.10319242789980509</v>
       </c>
@@ -2373,199 +2372,199 @@
       <c r="O42" s="1"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="F43" s="11" t="s">
+      <c r="C43" s="11"/>
+      <c r="F43" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G43" s="12"/>
-      <c r="J43" s="11" t="s">
+      <c r="G43" s="11"/>
+      <c r="J43" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K43" s="12"/>
-      <c r="N43" s="11" t="s">
+      <c r="K43" s="11"/>
+      <c r="N43" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O43" s="12"/>
+      <c r="O43" s="11"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="9">
         <f>_xlfn.VAR.P(C6:C7,C10:C11,C14:C15)</f>
         <v>0</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G44" s="9">
         <f>_xlfn.VAR.P(G6:G7,G10:G11,G14:G15)</f>
         <v>1.2222222222222223</v>
       </c>
-      <c r="J44" s="9" t="s">
+      <c r="J44" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K44" s="10">
+      <c r="K44" s="9">
         <f>_xlfn.VAR.P(K6:K7,K10:K11,K14:K15)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="N44" s="9" t="s">
+      <c r="N44" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O44" s="10">
+      <c r="O44" s="9">
         <f>_xlfn.VAR.P(O6:O7,O10:O11,O14:O15)</f>
         <v>4.4722222222222223</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="9">
         <f>_xlfn.VAR.P(C8:C9,C12:C13,C16:C17)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="10">
+      <c r="G45" s="9">
         <f>_xlfn.VAR.P(G8:G9,G12:G13,G16:G17)</f>
         <v>0</v>
       </c>
-      <c r="J45" s="9" t="s">
+      <c r="J45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K45" s="10">
+      <c r="K45" s="9">
         <f>_xlfn.VAR.P(K8:K9,K12:K13,K16:K17)</f>
         <v>0</v>
       </c>
-      <c r="N45" s="9" t="s">
+      <c r="N45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O45" s="10">
+      <c r="O45" s="9">
         <f>_xlfn.VAR.P(O8:O9,O12:O13,O16:O17)</f>
         <v>1.5833333333333333</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="9">
         <f>AVERAGE(C44:C45)</f>
         <v>0</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G46" s="10">
+      <c r="G46" s="9">
         <f>AVERAGE(G44:G45)</f>
         <v>0.61111111111111116</v>
       </c>
-      <c r="J46" s="9" t="s">
+      <c r="J46" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K46" s="10">
+      <c r="K46" s="9">
         <f>AVERAGE(K44:K45)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N46" s="9" t="s">
+      <c r="N46" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O46" s="10">
+      <c r="O46" s="9">
         <f>AVERAGE(O44:O45)</f>
         <v>3.0277777777777777</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="9">
         <f>AVERAGE(C22,C28,C34,C23,C29,C35)</f>
         <v>0</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G47" s="10">
+      <c r="G47" s="9">
         <f>AVERAGE(G22,G28,G34,G23,G29,G35)</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="J47" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K47" s="10">
+      <c r="K47" s="9">
         <f>AVERAGE(K22,K28,K34,K23,K29,K35)</f>
         <v>0</v>
       </c>
-      <c r="N47" s="9" t="s">
+      <c r="N47" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O47" s="10">
+      <c r="O47" s="9">
         <f>AVERAGE(O22,O28,O34,O23,O29,O35)</f>
         <v>2.25</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="9">
         <f>_xlfn.VAR.P(C6:C17)</f>
         <v>0</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G48" s="10">
+      <c r="G48" s="9">
         <f>_xlfn.VAR.P(G6:G17)</f>
         <v>1.9722222222222223</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="J48" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K48" s="10">
+      <c r="K48" s="9">
         <f>_xlfn.VAR.P(K6:K17)</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="N48" s="9" t="s">
+      <c r="N48" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O48" s="10">
+      <c r="O48" s="9">
         <f>_xlfn.VAR.P(O6:O17)</f>
         <v>3.0555555555555554</v>
       </c>
     </row>
     <row r="49" spans="2:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="16">
+      <c r="C49" s="15">
         <f>1-(((C46-C47)+$C$19)/((C48-C47)+$C$19))</f>
         <v>0</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G49" s="16">
+      <c r="G49" s="15">
         <f>1-(((G46-G47)+$C$19)/((G48-G47)+$C$19))</f>
         <v>0.72020694926215534</v>
       </c>
-      <c r="J49" s="15" t="s">
+      <c r="J49" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K49" s="16">
+      <c r="K49" s="15">
         <f>1-(((K46-K47)+$C$19)/((K48-K47)+$C$19))</f>
         <v>0.42783799201369088</v>
       </c>
-      <c r="N49" s="15" t="s">
+      <c r="N49" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="O49" s="16">
+      <c r="O49" s="15">
         <f>1-(((O46-O47)+$C$19)/((O48-O47)+$C$19))</f>
         <v>3.4440005510400717E-2</v>
       </c>

</xml_diff>